<commit_message>
Programing language: Java Technue used: - TestNG, Export Report, Maven Build Export Report : - Here screen shot is added at the end. In base class , Failure case is not working- Need to check it.
</commit_message>
<xml_diff>
--- a/FrameworkCreation/TestData/TestData.xlsx
+++ b/FrameworkCreation/TestData/TestData.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>jesmi</t>
+    <t>admin</t>
   </si>
   <si>
-    <t>admin</t>
+    <t>CHINNU</t>
+  </si>
+  <si>
+    <t>jesmi1</t>
   </si>
 </sst>
 </file>
@@ -358,11 +361,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -370,11 +371,14 @@
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>